<commit_message>
additional scraper functions added
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29304"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29307"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBDF28D1-ECE9-464B-8228-663AE728EA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6F2A06-B910-4794-8BC6-6326C763AD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="203">
   <si>
     <t>Type</t>
   </si>
@@ -665,6 +665,9 @@
   </si>
   <si>
     <t>no definite dates</t>
+  </si>
+  <si>
+    <t>timing issue on subpage</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1140,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A64" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G88" sqref="G88"/>
+      <selection activeCell="E96" sqref="E96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1183,7 +1186,7 @@
       </c>
       <c r="H2" s="7">
         <f>COUNTIF(D1:D1000, "WITH ISSUES")</f>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1225,7 +1228,7 @@
       </c>
       <c r="H4" s="11">
         <f>COUNTIF(D1:D1000, "COMPLETED")</f>
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1246,7 +1249,7 @@
       </c>
       <c r="H5" s="13">
         <f>COUNTIF(D1:D1000, "NOT YET COMPLETED")</f>
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2488,7 +2491,7 @@
         <v>194</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2498,11 +2501,11 @@
       <c r="B94" s="4" t="s">
         <v>195</v>
       </c>
-      <c r="C94" s="5" t="s">
+      <c r="C94" s="16" t="s">
         <v>196</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2512,11 +2515,14 @@
       <c r="B95" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="C95" s="5" t="s">
+      <c r="C95" s="16" t="s">
         <v>198</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>16</v>
+        <v>8</v>
+      </c>
+      <c r="E95" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added 2 new functions
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01A2BFDE-F80F-4232-99C2-FB4BBFFA9FB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6B19CE-6187-41A2-84D4-71463747F57A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="204">
   <si>
     <t>Type</t>
   </si>
@@ -668,6 +668,9 @@
   </si>
   <si>
     <t>messy classes</t>
+  </si>
+  <si>
+    <t>no explicit date used</t>
   </si>
 </sst>
 </file>
@@ -1139,8 +1142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1186,7 +1189,7 @@
       </c>
       <c r="H2" s="7">
         <f>COUNTIF(D1:D1000, "WITH ISSUES")</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1228,7 +1231,7 @@
       </c>
       <c r="H4" s="11">
         <f>COUNTIF(D1:D1000, "COMPLETED")</f>
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1249,7 +1252,7 @@
       </c>
       <c r="H5" s="13">
         <f>COUNTIF(D1:D1000, "NOT YET COMPLETED")</f>
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1413,7 +1416,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>4</v>
       </c>
@@ -1427,7 +1430,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
@@ -1441,7 +1444,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>4</v>
       </c>
@@ -1455,7 +1458,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>4</v>
       </c>
@@ -1469,7 +1472,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
@@ -1483,7 +1486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>4</v>
       </c>
@@ -1497,7 +1500,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
         <v>4</v>
       </c>
@@ -1508,10 +1511,10 @@
         <v>53</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>4</v>
       </c>
@@ -1525,35 +1528,38 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="C25" s="16" t="s">
         <v>57</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C26" s="16" t="s">
         <v>59</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>4</v>
       </c>
@@ -1567,7 +1573,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>4</v>
       </c>
@@ -1581,7 +1587,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>4</v>
       </c>
@@ -1595,7 +1601,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>4</v>
       </c>
@@ -1609,7 +1615,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>4</v>
       </c>
@@ -1623,7 +1629,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
applied fixes on functions
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A268852-CB10-49A3-8A44-D06CB31994D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C559E20-A9AF-4FA8-9E65-4F649E3256F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="2280" windowWidth="25155" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="397" uniqueCount="208">
   <si>
     <t>Type</t>
   </si>
@@ -680,6 +680,9 @@
   </si>
   <si>
     <t>Site is protected by Captcha</t>
+  </si>
+  <si>
+    <t>Updated</t>
   </si>
 </sst>
 </file>
@@ -849,7 +852,56 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59987182226020086"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59987182226020086"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1151,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G56" sqref="G56"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1243,7 @@
         <v>6</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>8</v>
@@ -1212,7 +1264,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>11</v>
@@ -1240,7 +1292,7 @@
       </c>
       <c r="H4" s="11">
         <f>COUNTIF(D1:D1000, "COMPLETED")</f>
-        <v>77</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1261,7 +1313,7 @@
       </c>
       <c r="H5" s="13">
         <f>COUNTIF(D1:D1000, "NOT YET COMPLETED")</f>
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1277,12 +1329,12 @@
       <c r="D6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="H6" s="12">
-        <f>SUM(H2:H5)</f>
-        <v>95</v>
+      <c r="G6" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="H6" s="13">
+        <f>COUNTIF(D2:D1001, "Updated")</f>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1298,6 +1350,13 @@
       <c r="D7" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="G7" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="H7" s="12">
+        <f>SUM(H2:H5)</f>
+        <v>75</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1310,7 +1369,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1411,7 +1470,7 @@
         <v>37</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1421,7 +1480,7 @@
       <c r="B16" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="16" t="s">
         <v>39</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -1453,7 +1512,7 @@
         <v>43</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1467,7 +1526,7 @@
         <v>45</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1509,7 +1568,7 @@
         <v>51</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1568,7 +1627,7 @@
         <v>59</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2039,7 +2098,7 @@
         <v>125</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2049,11 +2108,11 @@
       <c r="B60" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C60" s="16" t="s">
         <v>127</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -2063,11 +2122,11 @@
       <c r="B61" s="15" t="s">
         <v>128</v>
       </c>
-      <c r="C61" s="5" t="s">
+      <c r="C61" s="16" t="s">
         <v>129</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -2077,11 +2136,11 @@
       <c r="B62" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C62" s="5" t="s">
+      <c r="C62" s="16" t="s">
         <v>131</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2091,11 +2150,11 @@
       <c r="B63" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C63" s="16" t="s">
         <v>133</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2109,7 +2168,7 @@
         <v>135</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -2119,11 +2178,11 @@
       <c r="B65" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C65" s="5" t="s">
+      <c r="C65" s="16" t="s">
         <v>137</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -2133,11 +2192,11 @@
       <c r="B66" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C66" s="5" t="s">
+      <c r="C66" s="16" t="s">
         <v>139</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -2151,7 +2210,7 @@
         <v>142</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -2165,7 +2224,7 @@
         <v>144</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -2179,7 +2238,7 @@
         <v>146</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -2193,7 +2252,7 @@
         <v>148</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -2203,11 +2262,11 @@
       <c r="B71" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="C71" s="5" t="s">
+      <c r="C71" s="16" t="s">
         <v>150</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -2221,7 +2280,7 @@
         <v>152</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -2231,11 +2290,11 @@
       <c r="B73" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C73" s="16" t="s">
         <v>154</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -2249,7 +2308,7 @@
         <v>156</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2263,7 +2322,7 @@
         <v>158</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2277,7 +2336,7 @@
         <v>160</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2291,7 +2350,7 @@
         <v>162</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2305,7 +2364,7 @@
         <v>164</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2319,7 +2378,7 @@
         <v>166</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2333,7 +2392,7 @@
         <v>168</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2347,7 +2406,7 @@
         <v>170</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2361,7 +2420,7 @@
         <v>172</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2375,7 +2434,7 @@
         <v>174</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2389,7 +2448,7 @@
         <v>176</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2431,7 +2490,7 @@
         <v>182</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2473,7 +2532,7 @@
         <v>188</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2518,7 +2577,7 @@
         <v>194</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2563,41 +2622,47 @@
         <v>200</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:D95 A97:A1000 B98:D1000">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>$D2="Updated"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>$D2="Page Unresponsive"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>$D2="With Issues"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="5">
+    <cfRule type="expression" dxfId="3" priority="6">
       <formula>$D2="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D1000">
-    <cfRule type="expression" priority="4">
+    <cfRule type="expression" priority="5">
       <formula>$D2="Not Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:D97">
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>$D96="Page Unresponsive"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="7">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>$D96="With Issues"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="9">
+    <cfRule type="expression" dxfId="0" priority="10">
       <formula>$D96="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1:D96" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D1" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Completed,Not Yet Completed,Page Unresponsive,With Issues"</formula1>
       <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D96" xr:uid="{063F5AB0-2047-4156-ACED-713D3525561F}">
+      <formula1>"Completed,Not Yet Completed,Page Unresponsive,With Issues, Updated"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
@@ -2661,41 +2726,41 @@
     <hyperlink ref="C59" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
     <hyperlink ref="C60" r:id="rId59" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
     <hyperlink ref="C61" r:id="rId60" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="C62" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="C63" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="C64" r:id="rId63" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
-    <hyperlink ref="C65" r:id="rId64" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
-    <hyperlink ref="C66" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
-    <hyperlink ref="C67" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
-    <hyperlink ref="C68" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
-    <hyperlink ref="C69" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
-    <hyperlink ref="C70" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
-    <hyperlink ref="C71" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
-    <hyperlink ref="C72" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
-    <hyperlink ref="C73" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
-    <hyperlink ref="C74" r:id="rId73" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
-    <hyperlink ref="C75" r:id="rId74" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
-    <hyperlink ref="C76" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
-    <hyperlink ref="C77" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
-    <hyperlink ref="C78" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
-    <hyperlink ref="C79" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
-    <hyperlink ref="C80" r:id="rId79" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
-    <hyperlink ref="C81" r:id="rId80" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
-    <hyperlink ref="C82" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
-    <hyperlink ref="C83" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
-    <hyperlink ref="C84" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
-    <hyperlink ref="C85" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
-    <hyperlink ref="C86" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
-    <hyperlink ref="C87" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
-    <hyperlink ref="C88" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
-    <hyperlink ref="C89" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
-    <hyperlink ref="C90" r:id="rId89" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
-    <hyperlink ref="C91" r:id="rId90" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
-    <hyperlink ref="C92" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
-    <hyperlink ref="C93" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
-    <hyperlink ref="C94" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
-    <hyperlink ref="C95" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
-    <hyperlink ref="C96" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="C63" r:id="rId61" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="C65" r:id="rId62" xr:uid="{00000000-0004-0000-0000-00003F000000}"/>
+    <hyperlink ref="C66" r:id="rId63" xr:uid="{00000000-0004-0000-0000-000040000000}"/>
+    <hyperlink ref="C67" r:id="rId64" xr:uid="{00000000-0004-0000-0000-000041000000}"/>
+    <hyperlink ref="C68" r:id="rId65" xr:uid="{00000000-0004-0000-0000-000042000000}"/>
+    <hyperlink ref="C69" r:id="rId66" xr:uid="{00000000-0004-0000-0000-000043000000}"/>
+    <hyperlink ref="C70" r:id="rId67" xr:uid="{00000000-0004-0000-0000-000044000000}"/>
+    <hyperlink ref="C71" r:id="rId68" xr:uid="{00000000-0004-0000-0000-000045000000}"/>
+    <hyperlink ref="C72" r:id="rId69" xr:uid="{00000000-0004-0000-0000-000046000000}"/>
+    <hyperlink ref="C73" r:id="rId70" xr:uid="{00000000-0004-0000-0000-000047000000}"/>
+    <hyperlink ref="C74" r:id="rId71" xr:uid="{00000000-0004-0000-0000-000048000000}"/>
+    <hyperlink ref="C75" r:id="rId72" xr:uid="{00000000-0004-0000-0000-000049000000}"/>
+    <hyperlink ref="C76" r:id="rId73" xr:uid="{00000000-0004-0000-0000-00004A000000}"/>
+    <hyperlink ref="C77" r:id="rId74" xr:uid="{00000000-0004-0000-0000-00004B000000}"/>
+    <hyperlink ref="C78" r:id="rId75" xr:uid="{00000000-0004-0000-0000-00004C000000}"/>
+    <hyperlink ref="C79" r:id="rId76" xr:uid="{00000000-0004-0000-0000-00004D000000}"/>
+    <hyperlink ref="C80" r:id="rId77" xr:uid="{00000000-0004-0000-0000-00004E000000}"/>
+    <hyperlink ref="C81" r:id="rId78" xr:uid="{00000000-0004-0000-0000-00004F000000}"/>
+    <hyperlink ref="C82" r:id="rId79" xr:uid="{00000000-0004-0000-0000-000050000000}"/>
+    <hyperlink ref="C83" r:id="rId80" xr:uid="{00000000-0004-0000-0000-000051000000}"/>
+    <hyperlink ref="C84" r:id="rId81" xr:uid="{00000000-0004-0000-0000-000052000000}"/>
+    <hyperlink ref="C85" r:id="rId82" xr:uid="{00000000-0004-0000-0000-000053000000}"/>
+    <hyperlink ref="C86" r:id="rId83" xr:uid="{00000000-0004-0000-0000-000054000000}"/>
+    <hyperlink ref="C87" r:id="rId84" xr:uid="{00000000-0004-0000-0000-000055000000}"/>
+    <hyperlink ref="C88" r:id="rId85" xr:uid="{00000000-0004-0000-0000-000056000000}"/>
+    <hyperlink ref="C89" r:id="rId86" xr:uid="{00000000-0004-0000-0000-000057000000}"/>
+    <hyperlink ref="C90" r:id="rId87" xr:uid="{00000000-0004-0000-0000-000058000000}"/>
+    <hyperlink ref="C91" r:id="rId88" xr:uid="{00000000-0004-0000-0000-000059000000}"/>
+    <hyperlink ref="C92" r:id="rId89" xr:uid="{00000000-0004-0000-0000-00005A000000}"/>
+    <hyperlink ref="C93" r:id="rId90" xr:uid="{00000000-0004-0000-0000-00005B000000}"/>
+    <hyperlink ref="C94" r:id="rId91" xr:uid="{00000000-0004-0000-0000-00005C000000}"/>
+    <hyperlink ref="C95" r:id="rId92" xr:uid="{00000000-0004-0000-0000-00005D000000}"/>
+    <hyperlink ref="C96" r:id="rId93" xr:uid="{00000000-0004-0000-0000-00005E000000}"/>
+    <hyperlink ref="C62" r:id="rId94" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="C64" r:id="rId95" xr:uid="{00000000-0004-0000-0000-00003E000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId96"/>

</xml_diff>

<commit_message>
latest version,, function improvements applied
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29318"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96C0B81-3A9B-4F4F-AC7D-7829EA57CE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26B0AE6-EED4-45C7-8FDA-D2069A609AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2055" yWindow="1485" windowWidth="25155" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -860,7 +860,35 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79989013336588644"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59987182226020086"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1169,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D94" sqref="D94"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1279,7 +1307,7 @@
       </c>
       <c r="H5" s="12">
         <f>COUNTIF(D1:D1000, "NOT YET COMPLETED")</f>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1300,7 +1328,7 @@
       </c>
       <c r="H6" s="12">
         <f>COUNTIF(D2:D1001, "Updated")</f>
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1321,7 +1349,7 @@
       </c>
       <c r="H7" s="11">
         <f>SUM(H2:H5)</f>
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2538,7 +2566,7 @@
         <v>192</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>16</v>
+        <v>207</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2552,7 +2580,7 @@
         <v>194</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>16</v>
+        <v>207</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2566,7 +2594,7 @@
         <v>196</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>16</v>
+        <v>207</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2597,37 +2625,51 @@
         <v>200</v>
       </c>
       <c r="D96" s="2" t="s">
-        <v>16</v>
+        <v>207</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:D95 A97:A1000 B98:D1000">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>$D2="Updated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="9" priority="7">
       <formula>$D2="Page Unresponsive"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>$D2="With Issues"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="6">
+    <cfRule type="expression" dxfId="7" priority="10">
       <formula>$D2="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2:D1000">
-    <cfRule type="expression" priority="5">
+    <cfRule type="expression" priority="9">
       <formula>$D2="Not Completed"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:D97">
-    <cfRule type="expression" dxfId="2" priority="7">
+    <cfRule type="expression" dxfId="6" priority="11">
       <formula>$D96="Page Unresponsive"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="8">
+    <cfRule type="expression" dxfId="5" priority="12">
       <formula>$D96="With Issues"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="10">
+    <cfRule type="expression" dxfId="4" priority="14">
+      <formula>$D96="Completed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A96:D96">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$D96="Updated"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>$D96="Page Unresponsive"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="3">
+      <formula>$D96="With Issues"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="4">
       <formula>$D96="Completed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
continuation of applied fixes
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29318"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29322"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F26B0AE6-EED4-45C7-8FDA-D2069A609AC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F966A0-2D95-45E8-BEA8-6E84A3C59F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="1485" windowWidth="25155" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -885,13 +885,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor theme="9" tint="0.79989013336588644"/>
         </patternFill>
       </fill>
@@ -907,6 +900,13 @@
       <fill>
         <patternFill>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="H5" s="12">
         <f>COUNTIF(D1:D1000, "NOT YET COMPLETED")</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="H6" s="12">
         <f>COUNTIF(D2:D1001, "Updated")</f>
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="H7" s="11">
         <f>SUM(H2:H5)</f>
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1363,7 +1363,7 @@
         <v>23</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>16</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1506,7 +1506,7 @@
         <v>43</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>16</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2629,17 +2629,31 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:D95 A97:A1000 B98:D1000">
+  <conditionalFormatting sqref="A97:A1000 B98:D1000">
     <cfRule type="expression" dxfId="10" priority="5">
+      <formula>$D97="Updated"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="9" priority="7">
+      <formula>$D97="Page Unresponsive"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="8">
+      <formula>$D97="With Issues"</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="10">
+      <formula>$D97="Completed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:D96">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>$D2="Updated"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="7">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>$D2="Page Unresponsive"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="8">
+    <cfRule type="expression" dxfId="4" priority="3">
       <formula>$D2="With Issues"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="10">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$D2="Completed"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2649,27 +2663,13 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A96:D97">
-    <cfRule type="expression" dxfId="6" priority="11">
+    <cfRule type="expression" dxfId="2" priority="11">
       <formula>$D96="Page Unresponsive"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="12">
+    <cfRule type="expression" dxfId="1" priority="12">
       <formula>$D96="With Issues"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="14">
-      <formula>$D96="Completed"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A96:D96">
-    <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$D96="Updated"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>$D96="Page Unresponsive"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="3">
-      <formula>$D96="With Issues"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="4">
+    <cfRule type="expression" dxfId="0" priority="14">
       <formula>$D96="Completed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
updated functions - minor fixes
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28F966A0-2D95-45E8-BEA8-6E84A3C59F69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A32CEFCE-ACF5-4B9D-BE47-0313F2E2B6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="209">
   <si>
     <t>Type</t>
   </si>
@@ -1197,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G73" sqref="G73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1941,7 +1941,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>4</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>4</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>4</v>
       </c>
@@ -1983,7 +1983,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>4</v>
       </c>
@@ -1997,7 +1997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>4</v>
       </c>
@@ -2011,7 +2011,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>4</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>4</v>
       </c>
@@ -2039,7 +2039,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>4</v>
       </c>
@@ -2052,8 +2052,11 @@
       <c r="D56" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>4</v>
       </c>
@@ -2067,7 +2070,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>4</v>
       </c>
@@ -2081,7 +2084,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>4</v>
       </c>
@@ -2095,7 +2098,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>4</v>
       </c>
@@ -2109,7 +2112,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>4</v>
       </c>
@@ -2123,7 +2126,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>4</v>
       </c>
@@ -2137,7 +2140,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>4</v>
       </c>
@@ -2151,7 +2154,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>4</v>
       </c>
@@ -2163,6 +2166,9 @@
       </c>
       <c r="D64" s="2" t="s">
         <v>7</v>
+      </c>
+      <c r="E64" s="17" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added new functions with previous issues
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E4E1FB2-AE35-4C6B-8838-66CE9E9E75DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{016613EB-10B1-42E3-9B28-D60B4B4ACA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2055" yWindow="1485" windowWidth="25155" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1194,8 +1194,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F88" sqref="F88"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1241,7 +1241,7 @@
       </c>
       <c r="H2" s="6">
         <f>COUNTIF(D1:D1000, "WITH ISSUES")</f>
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1325,7 +1325,7 @@
       </c>
       <c r="H6" s="12">
         <f>COUNTIF(D2:D1001, "Updated")</f>
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1346,7 +1346,7 @@
       </c>
       <c r="H7" s="11">
         <f>SUM(H2:H5)</f>
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1374,7 +1374,7 @@
         <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>8</v>
+        <v>206</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
continued update of functions
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python_Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBAC78D-B12A-4214-BE93-032504F71695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523E2DB8-E531-4E19-9638-03DDB0229424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="9960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1198,7 +1198,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="H4" s="10">
         <f>COUNTIF(D1:D1000, "COMPLETED")</f>
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="H6" s="12">
         <f>COUNTIF(D2:D1001, "Updated")</f>
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="H7" s="11">
         <f>SUM(H2:H5)</f>
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1405,7 +1405,7 @@
         <v>29</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>7</v>
+        <v>205</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated a new function
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python_Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10BC4510-E1DB-443E-AB8A-7FC971CC772E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0022E8C5-ABE3-4AB9-9E4F-AAD4E7202B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1198,20 +1198,20 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.140625" customWidth="1"/>
-    <col min="2" max="2" width="50.28515625" customWidth="1"/>
-    <col min="3" max="3" width="61.7109375" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5703125" style="17" customWidth="1"/>
-    <col min="7" max="7" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" width="14.109375" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" customWidth="1"/>
+    <col min="3" max="3" width="61.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5546875" style="17" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1289,7 +1289,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1310,7 +1310,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
@@ -1467,7 +1467,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>4</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>4</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>4</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>4</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>4</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>4</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>4</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>4</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>4</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>4</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>4</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>4</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>4</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>4</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>4</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>4</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>4</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>4</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>4</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>4</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>4</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>4</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>4</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>4</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>4</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>4</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>4</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>4</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>4</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>4</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>4</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>4</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>4</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>4</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>4</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>4</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>4</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>4</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>4</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>4</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>4</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>140</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>140</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>140</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>140</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>140</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>140</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>140</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>140</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>140</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>140</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>140</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>140</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>140</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>140</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>140</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>140</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>140</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>140</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>140</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>140</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>140</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>140</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>140</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>140</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>140</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>140</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>140</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>140</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>140</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>140</v>
       </c>

</xml_diff>

<commit_message>
continued refactor of functions
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Python_Projects\HVAC_News_Scraper\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0022E8C5-ABE3-4AB9-9E4F-AAD4E7202B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF43386C-C84A-4915-852F-44EA73261D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="9960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1198,20 +1198,20 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.109375" customWidth="1"/>
-    <col min="2" max="2" width="50.33203125" customWidth="1"/>
-    <col min="3" max="3" width="61.6640625" customWidth="1"/>
-    <col min="4" max="4" width="24.5546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.5546875" style="17" customWidth="1"/>
-    <col min="7" max="7" width="33.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="50.28515625" customWidth="1"/>
+    <col min="3" max="3" width="61.7109375" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="E1" s="16"/>
     </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -1286,10 +1286,10 @@
       </c>
       <c r="H4" s="10">
         <f>COUNTIF(D1:D1000, "COMPLETED")</f>
-        <v>44</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1307,10 +1307,10 @@
       </c>
       <c r="H5" s="12">
         <f>COUNTIF(D1:D1000, "NOT YET COMPLETED")</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1328,10 +1328,10 @@
       </c>
       <c r="H6" s="12">
         <f>COUNTIF(D2:D1001, "Updated")</f>
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>4</v>
       </c>
@@ -1349,10 +1349,10 @@
       </c>
       <c r="H7" s="11">
         <f>SUM(H2:H5)</f>
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>4</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>4</v>
       </c>
@@ -1408,7 +1408,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>4</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>4</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>4</v>
       </c>
@@ -1450,24 +1450,24 @@
         <v>35</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="C15" s="15" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>4</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
@@ -1509,7 +1509,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
@@ -1523,7 +1523,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
@@ -1537,7 +1537,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
@@ -1551,7 +1551,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>4</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>4</v>
       </c>
@@ -1579,7 +1579,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>4</v>
       </c>
@@ -1593,7 +1593,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>4</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>4</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>4</v>
       </c>
@@ -1649,7 +1649,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>4</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>4</v>
       </c>
@@ -1677,7 +1677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>4</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>4</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>4</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>4</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>4</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>4</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>4</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>4</v>
       </c>
@@ -1798,7 +1798,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>4</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>4</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>4</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>4</v>
       </c>
@@ -1854,7 +1854,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>4</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>4</v>
       </c>
@@ -1882,7 +1882,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>4</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>4</v>
       </c>
@@ -1910,7 +1910,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>4</v>
       </c>
@@ -1924,7 +1924,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>4</v>
       </c>
@@ -1938,7 +1938,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>4</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>4</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>4</v>
       </c>
@@ -1980,7 +1980,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>4</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>4</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>4</v>
       </c>
@@ -2022,7 +2022,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>4</v>
       </c>
@@ -2036,7 +2036,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>4</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>4</v>
       </c>
@@ -2067,7 +2067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>4</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>4</v>
       </c>
@@ -2095,7 +2095,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>4</v>
       </c>
@@ -2109,7 +2109,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>4</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>4</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>4</v>
       </c>
@@ -2151,7 +2151,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>4</v>
       </c>
@@ -2168,7 +2168,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>4</v>
       </c>
@@ -2182,7 +2182,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>4</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>140</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>140</v>
       </c>
@@ -2224,7 +2224,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>140</v>
       </c>
@@ -2238,7 +2238,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>140</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>140</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>140</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>140</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>140</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>140</v>
       </c>
@@ -2331,7 +2331,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>140</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>140</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>140</v>
       </c>
@@ -2373,7 +2373,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>140</v>
       </c>
@@ -2387,7 +2387,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>140</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>140</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>140</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="83" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>140</v>
       </c>
@@ -2443,7 +2443,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="84" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>140</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="85" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>140</v>
       </c>
@@ -2471,7 +2471,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>140</v>
       </c>
@@ -2485,7 +2485,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>140</v>
       </c>
@@ -2499,7 +2499,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>140</v>
       </c>
@@ -2516,7 +2516,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>140</v>
       </c>
@@ -2530,7 +2530,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>140</v>
       </c>
@@ -2544,7 +2544,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="91" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>140</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>140</v>
       </c>
@@ -2575,7 +2575,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="93" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>140</v>
       </c>
@@ -2589,7 +2589,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>140</v>
       </c>
@@ -2603,7 +2603,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>140</v>
       </c>
@@ -2620,7 +2620,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>140</v>
       </c>

</xml_diff>

<commit_message>
refactored another scraper function
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29413"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF43386C-C84A-4915-852F-44EA73261D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A232298C-E886-4D05-B3FF-1B4D8B161E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1198,7 +1198,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="H4" s="10">
         <f>COUNTIF(D1:D1000, "COMPLETED")</f>
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="H6" s="12">
         <f>COUNTIF(D2:D1001, "Updated")</f>
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="H7" s="11">
         <f>SUM(H2:H5)</f>
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1492,7 +1492,7 @@
         <v>41</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>7</v>
+        <v>205</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
continued to refactor function
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A232298C-E886-4D05-B3FF-1B4D8B161E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2231FC83-9D12-4526-A839-9D836E74D054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1198,7 +1198,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="H5" s="12">
         <f>COUNTIF(D1:D1000, "NOT YET COMPLETED")</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="H6" s="12">
         <f>COUNTIF(D2:D1001, "Updated")</f>
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="H7" s="11">
         <f>SUM(H2:H5)</f>
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1520,7 +1520,7 @@
         <v>45</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>16</v>
+        <v>205</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
continued to refactor functions
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B240E1-D980-46C1-957B-AEB25216EEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C17BADC-B1E6-4B82-B157-A1066BCC3391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="3015" windowWidth="25620" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1198,7 +1198,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="H4" s="10">
         <f>COUNTIF(D1:D1000, "COMPLETED")</f>
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="H6" s="12">
         <f>COUNTIF(D2:D1001, "Updated")</f>
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="H7" s="11">
         <f>SUM(H2:H5)</f>
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1534,7 +1534,7 @@
         <v>47</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>7</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
refactored old non-working function
</commit_message>
<xml_diff>
--- a/assets/Sources.xlsx
+++ b/assets/Sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\HVAC_News_Scraper\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C17BADC-B1E6-4B82-B157-A1066BCC3391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F033C7B3-E109-404D-8523-C7D0665C5146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1198,7 +1198,7 @@
   <dimension ref="A1:H96"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="H4" s="10">
         <f>COUNTIF(D1:D1000, "COMPLETED")</f>
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="H6" s="12">
         <f>COUNTIF(D2:D1001, "Updated")</f>
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1349,7 +1349,7 @@
       </c>
       <c r="H7" s="11">
         <f>SUM(H2:H5)</f>
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1548,7 +1548,7 @@
         <v>49</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>7</v>
+        <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>